<commit_message>
Snackbar, Visitor, About, Skills Spinner, Accent Coloring
</commit_message>
<xml_diff>
--- a/data/xlsx/education.xlsx
+++ b/data/xlsx/education.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wheel\WebstormProjects\CloudGuruChallenge_21.04\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFF8ACF-97A4-4B6E-911B-3CC5351A8AC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940AFA42-2BBD-409E-BD17-1F0094D17C61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -37,18 +37,12 @@
     <t>degree</t>
   </si>
   <si>
-    <t>end_year</t>
-  </si>
-  <si>
     <t>field</t>
   </si>
   <si>
     <t>Game Design and Development</t>
   </si>
   <si>
-    <t>start_year</t>
-  </si>
-  <si>
     <t>Bachelor of Science</t>
   </si>
   <si>
@@ -74,6 +68,12 @@
   </si>
   <si>
     <t>Florida</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>start</t>
   </si>
 </sst>
 </file>
@@ -966,7 +966,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -996,28 +996,28 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1025,7 +1025,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -1034,19 +1034,19 @@
         <v>2016</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J2" s="5">
         <v>32792</v>

</xml_diff>

<commit_message>
Education.descriptions and Education Data
</commit_message>
<xml_diff>
--- a/data/xlsx/education.xlsx
+++ b/data/xlsx/education.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wheel\WebstormProjects\CloudGuruChallenge_21.04\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940AFA42-2BBD-409E-BD17-1F0094D17C61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652F71B5-10B0-4548-AA0F-4023D69E29A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -22,15 +22,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Mauris venenatis purus ac mauris vehicula, tristique tempor tellus lobortis. Fusce semper eu elit ac elementum. Aenean tincidunt venenatis nisl, at egestas massa ullamcorper at. Maecenas dui ex, egestas at velit eu, dictum tempor dolor. Donec varius ac nisi sit amet ultrices.</t>
-  </si>
-  <si>
     <t>Full Sail University</t>
   </si>
   <si>
@@ -74,6 +68,18 @@
   </si>
   <si>
     <t>start</t>
+  </si>
+  <si>
+    <t>descriptions</t>
+  </si>
+  <si>
+    <t>[
+"Created a board game to simulate skills without coding",
+"Created story boards to illustrate the user's experience",
+"Designed and implemented virtual worlds using the Unity game engine",
+"Developed believable physics, partical effects, reward system, and state machine logic",
+"Learned about history, psychology, math, mythology, and science in relation to Game Design"
+]</t>
   </si>
 </sst>
 </file>
@@ -591,7 +597,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -607,6 +613,15 @@
     </xf>
     <xf numFmtId="1" fontId="19" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -965,15 +980,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="8" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
@@ -985,68 +1000,68 @@
     <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D2" s="5">
         <v>2016</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J2" s="5">
         <v>32792</v>

</xml_diff>

<commit_message>
Updated Web Backend to use Environment, Data Changes, Terraform for Cloud Run Domain Mapping
</commit_message>
<xml_diff>
--- a/data/xlsx/education.xlsx
+++ b/data/xlsx/education.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wheel\WebstormProjects\CloudGuruChallenge_21.04\data\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wheel\WebstormProjects\Resume\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652F71B5-10B0-4548-AA0F-4023D69E29A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45EF585-289A-408B-9C94-9A48ED27A583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -80,6 +80,12 @@
 "Developed believable physics, partical effects, reward system, and state machine logic",
 "Learned about history, psychology, math, mythology, and science in relation to Game Design"
 ]</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>eedfd009-a800-4426-95b8-1bc2251dbeb9</t>
   </si>
 </sst>
 </file>
@@ -978,95 +984,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="40.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5">
+      <c r="E2" s="5">
         <v>2016</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="b">
+      <c r="I2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="5">
+      <c r="K2" s="5">
         <v>32792</v>
       </c>
-      <c r="K2" s="5">
+      <c r="L2" s="5">
         <v>2013</v>
       </c>
     </row>

</xml_diff>